<commit_message>
HW1 update finfish 5
完成第5個功能
但是第一個功能的first <= second的部分還是有問題
</commit_message>
<xml_diff>
--- a/test0.xlsx
+++ b/test0.xlsx
@@ -17,9 +17,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -45,6 +45,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -56,13 +63,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -108,12 +108,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="新細明體"/>
@@ -121,16 +144,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,22 +155,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="新細明體"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="新細明體"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,19 +183,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -207,7 +285,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,31 +309,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,25 +333,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,85 +357,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,6 +411,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -425,17 +440,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -457,17 +468,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -482,7 +482,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -491,7 +491,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -500,127 +500,127 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -942,15 +942,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="16.2" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="16.2" outlineLevelRow="4" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>1</v>
       </c>
@@ -963,8 +963,11 @@
       <c r="D1">
         <v>12</v>
       </c>
+      <c r="E1">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>4</v>
       </c>
@@ -977,8 +980,11 @@
       <c r="D2">
         <v>45</v>
       </c>
+      <c r="E2">
+        <v>46</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>9</v>
       </c>
@@ -990,6 +996,43 @@
       </c>
       <c r="D3">
         <v>13</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>16.5</v>
+      </c>
+      <c r="E5">
+        <v>15.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>